<commit_message>
Bug Fix & August Data
Fixed a bug where program would terminate if item was missing a title. Completed data scrape for August.
</commit_message>
<xml_diff>
--- a/ebay_scraper.xlsx
+++ b/ebay_scraper.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Romek\Desktop\ebay scraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D26FFBD-E490-444D-877F-FBB89B2C160E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5550F0B2-B59C-4FDE-90E4-5C3C286788CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="0" windowWidth="20505" windowHeight="13080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw_data" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="240">
   <si>
     <t>Title</t>
   </si>
@@ -68,97 +69,613 @@
     <t>Month</t>
   </si>
   <si>
+    <t>Mountain</t>
+  </si>
+  <si>
+    <t>August</t>
+  </si>
+  <si>
+    <t>Start Row</t>
+  </si>
+  <si>
+    <t>2xl</t>
+  </si>
+  <si>
+    <t>Current Month</t>
+  </si>
+  <si>
+    <t>Xl</t>
+  </si>
+  <si>
+    <t>Times Ran (mth)</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Wolf</t>
+  </si>
+  <si>
+    <t>Graphic</t>
+  </si>
+  <si>
+    <t>Tank</t>
+  </si>
+  <si>
+    <t>Top</t>
+  </si>
+  <si>
+    <t>Surf</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Sided</t>
+  </si>
+  <si>
+    <t>Print</t>
+  </si>
+  <si>
+    <t>Yellow</t>
+  </si>
+  <si>
+    <t>X-large</t>
+  </si>
+  <si>
+    <t>90's</t>
+  </si>
+  <si>
+    <t>Marlboro</t>
+  </si>
+  <si>
+    <t>Pocket</t>
+  </si>
+  <si>
+    <t>Stitch</t>
+  </si>
+  <si>
+    <t>Wwe</t>
+  </si>
+  <si>
+    <t>Punk</t>
+  </si>
+  <si>
+    <t>Wrestling</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Big</t>
+  </si>
+  <si>
+    <t>Large</t>
+  </si>
+  <si>
+    <t>Nwt</t>
+  </si>
+  <si>
+    <t>Harley</t>
+  </si>
+  <si>
+    <t>Davidson</t>
+  </si>
+  <si>
+    <t>Beach</t>
+  </si>
+  <si>
+    <t>Usa</t>
+  </si>
+  <si>
+    <t>Made</t>
+  </si>
+  <si>
+    <t>Distressed</t>
+  </si>
+  <si>
+    <t>70s</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>1988</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>80s</t>
+  </si>
+  <si>
+    <t>Art</t>
+  </si>
+  <si>
+    <t>Majestic</t>
+  </si>
+  <si>
+    <t>Nfl</t>
+  </si>
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>Jersey</t>
+  </si>
+  <si>
+    <t>90s</t>
+  </si>
+  <si>
+    <t>Dead</t>
+  </si>
+  <si>
+    <t>80’s</t>
+  </si>
+  <si>
+    <t>Grateful</t>
+  </si>
+  <si>
+    <t>Lot</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>1997</t>
+  </si>
+  <si>
+    <t>Champions</t>
+  </si>
+  <si>
+    <t>Korn</t>
+  </si>
+  <si>
+    <t>Tour</t>
+  </si>
+  <si>
+    <t>Concert</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>Rock</t>
+  </si>
+  <si>
+    <t>Metal</t>
+  </si>
+  <si>
+    <t>University</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>1990</t>
+  </si>
+  <si>
+    <t>Nba</t>
+  </si>
+  <si>
+    <t>World</t>
+  </si>
+  <si>
+    <t>Screen</t>
+  </si>
+  <si>
+    <t>Stars</t>
+  </si>
+  <si>
+    <t>Best</t>
+  </si>
+  <si>
+    <t>1994</t>
+  </si>
+  <si>
+    <t>Cartoon</t>
+  </si>
+  <si>
+    <t>San</t>
+  </si>
+  <si>
+    <t>Logo</t>
+  </si>
+  <si>
+    <t>Grey</t>
+  </si>
+  <si>
+    <t>Original</t>
+  </si>
+  <si>
+    <t>Up</t>
+  </si>
+  <si>
+    <t>With</t>
+  </si>
+  <si>
+    <t>Navy</t>
+  </si>
+  <si>
+    <t>Jesus</t>
+  </si>
+  <si>
+    <t>Short</t>
+  </si>
+  <si>
+    <t>Sleeve</t>
+  </si>
+  <si>
+    <t>1987</t>
+  </si>
+  <si>
+    <t>1996</t>
+  </si>
+  <si>
+    <t>Tie</t>
+  </si>
+  <si>
+    <t>Dye</t>
+  </si>
+  <si>
+    <t>Double</t>
+  </si>
+  <si>
+    <t>Skateboards</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>Skull</t>
+  </si>
+  <si>
+    <t>Neck</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>Pink</t>
+  </si>
+  <si>
+    <t>Brockum</t>
+  </si>
+  <si>
+    <t>1980s</t>
+  </si>
+  <si>
+    <t>York</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>2000s</t>
+  </si>
+  <si>
+    <t>Gildan</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>Wwf</t>
+  </si>
+  <si>
+    <t>Rare</t>
+  </si>
+  <si>
+    <t>Camel</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Fruit</t>
+  </si>
+  <si>
+    <t>Loom</t>
+  </si>
+  <si>
+    <t>Anvil</t>
+  </si>
+  <si>
+    <t>Small</t>
+  </si>
+  <si>
+    <t>Stussy</t>
+  </si>
+  <si>
+    <t>1998</t>
+  </si>
+  <si>
+    <t>Rap</t>
+  </si>
+  <si>
+    <t>2003</t>
+  </si>
+  <si>
+    <t>Disney</t>
+  </si>
+  <si>
+    <t>Movie</t>
+  </si>
+  <si>
+    <t>Giant</t>
+  </si>
+  <si>
+    <t>Faded</t>
+  </si>
+  <si>
+    <t>Y2k</t>
+  </si>
+  <si>
+    <t>Long</t>
+  </si>
+  <si>
+    <t>Eagle</t>
+  </si>
+  <si>
+    <t>Biker</t>
+  </si>
+  <si>
     <t>American</t>
   </si>
   <si>
-    <t>August</t>
-  </si>
-  <si>
-    <t>Start Row</t>
-  </si>
-  <si>
-    <t>Eagle</t>
-  </si>
-  <si>
-    <t>Current Month</t>
-  </si>
-  <si>
-    <t>Wolf</t>
-  </si>
-  <si>
-    <t>Times Ran (mth)</t>
-  </si>
-  <si>
-    <t>2xl</t>
-  </si>
-  <si>
-    <t>Double</t>
-  </si>
-  <si>
-    <t>Sided</t>
-  </si>
-  <si>
-    <t>Pride</t>
-  </si>
-  <si>
-    <t>Premium</t>
-  </si>
-  <si>
-    <t>Tri</t>
-  </si>
-  <si>
-    <t>Blend</t>
-  </si>
-  <si>
-    <t>Political</t>
-  </si>
-  <si>
-    <t>Long</t>
-  </si>
-  <si>
-    <t>Sleeve</t>
+    <t>1993</t>
+  </si>
+  <si>
+    <t>Hip</t>
+  </si>
+  <si>
+    <t>Hop</t>
+  </si>
+  <si>
+    <t>Liquid</t>
   </si>
   <si>
     <t>Over</t>
   </si>
   <si>
-    <t>Flag</t>
-  </si>
-  <si>
-    <t>Is</t>
-  </si>
-  <si>
-    <t>Graphic</t>
-  </si>
-  <si>
-    <t>Day</t>
+    <t>1991</t>
+  </si>
+  <si>
+    <t>Album</t>
+  </si>
+  <si>
+    <t>Youth</t>
+  </si>
+  <si>
+    <t>90’s</t>
+  </si>
+  <si>
+    <t>Looney</t>
+  </si>
+  <si>
+    <t>Tunes</t>
+  </si>
+  <si>
+    <t>Taz</t>
+  </si>
+  <si>
+    <t>Animal</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Music</t>
+  </si>
+  <si>
+    <t>Funny</t>
+  </si>
+  <si>
+    <t>Dog</t>
+  </si>
+  <si>
+    <t>Polo</t>
+  </si>
+  <si>
+    <t>Ralph</t>
+  </si>
+  <si>
+    <t>Lauren</t>
+  </si>
+  <si>
+    <t>Promo</t>
+  </si>
+  <si>
+    <t>Retro</t>
+  </si>
+  <si>
+    <t>Style</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Band</t>
+  </si>
+  <si>
+    <t>One</t>
+  </si>
+  <si>
+    <t>Skateboard</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Air</t>
+  </si>
+  <si>
+    <t>Aop</t>
+  </si>
+  <si>
+    <t>Bootleg</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>00s</t>
+  </si>
+  <si>
+    <t>Car</t>
+  </si>
+  <si>
+    <t>Adult</t>
+  </si>
+  <si>
+    <t>Extra</t>
+  </si>
+  <si>
+    <t>Out</t>
+  </si>
+  <si>
+    <t>Ringer</t>
   </si>
   <si>
     <t>Love</t>
   </si>
   <si>
-    <t>Large</t>
-  </si>
-  <si>
-    <t>Print</t>
-  </si>
-  <si>
-    <t>Xl</t>
-  </si>
-  <si>
-    <t>Dog</t>
-  </si>
-  <si>
-    <t>Short</t>
-  </si>
-  <si>
-    <t>Up</t>
+    <t>Nike</t>
+  </si>
+  <si>
+    <t>Unisex</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>Park</t>
+  </si>
+  <si>
+    <t>Classic</t>
+  </si>
+  <si>
+    <t>Football</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t>Racing</t>
+  </si>
+  <si>
+    <t>1995</t>
+  </si>
+  <si>
+    <t>Nascar</t>
+  </si>
+  <si>
+    <t>1992</t>
+  </si>
+  <si>
+    <t>Spellout</t>
+  </si>
+  <si>
+    <t>Skate</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>100%</t>
+  </si>
+  <si>
+    <t>Cotton</t>
+  </si>
+  <si>
+    <t>Basketball</t>
+  </si>
+  <si>
+    <t>Mann</t>
+  </si>
+  <si>
+    <t>Show</t>
+  </si>
+  <si>
+    <t>80's</t>
+  </si>
+  <si>
+    <t>Motorcycle</t>
+  </si>
+  <si>
+    <t>Hanes</t>
+  </si>
+  <si>
+    <t>2001</t>
+  </si>
+  <si>
+    <t>Yankees</t>
+  </si>
+  <si>
+    <t>Gray</t>
+  </si>
+  <si>
+    <t>Jordan</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Baseball</t>
+  </si>
+  <si>
+    <t>1989</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>Embroidered</t>
+  </si>
+  <si>
+    <t>Star</t>
+  </si>
+  <si>
+    <t>Wars</t>
+  </si>
+  <si>
+    <t>Mlb</t>
+  </si>
+  <si>
+    <t>Atlanta</t>
+  </si>
+  <si>
+    <t>Olympics</t>
+  </si>
+  <si>
+    <t>Us</t>
+  </si>
+  <si>
+    <t>Tv</t>
+  </si>
+  <si>
+    <t>Stone</t>
   </si>
   <si>
     <t>1990s</t>
   </si>
   <si>
-    <t>Red</t>
+    <t>Great</t>
+  </si>
+  <si>
+    <t>Old</t>
+  </si>
+  <si>
+    <t>Space</t>
+  </si>
+  <si>
+    <t>2005</t>
+  </si>
+  <si>
+    <t>Nature</t>
   </si>
   <si>
     <t>Mickey</t>
@@ -167,460 +684,100 @@
     <t>Mouse</t>
   </si>
   <si>
-    <t>Usa</t>
-  </si>
-  <si>
-    <t>Made</t>
-  </si>
-  <si>
-    <t>Stitch</t>
-  </si>
-  <si>
-    <t>80s</t>
-  </si>
-  <si>
-    <t>Gray</t>
-  </si>
-  <si>
-    <t>Promo</t>
-  </si>
-  <si>
-    <t>World</t>
-  </si>
-  <si>
-    <t>Tour</t>
-  </si>
-  <si>
-    <t>Rare</t>
-  </si>
-  <si>
-    <t>Black</t>
-  </si>
-  <si>
-    <t>1998</t>
-  </si>
-  <si>
-    <t>Blue</t>
-  </si>
-  <si>
-    <t>Classic</t>
-  </si>
-  <si>
-    <t>Retro</t>
-  </si>
-  <si>
-    <t>Pink</t>
-  </si>
-  <si>
-    <t>Biker</t>
-  </si>
-  <si>
-    <t>Logo</t>
+    <t>3xl</t>
+  </si>
+  <si>
+    <t>1999</t>
+  </si>
+  <si>
+    <t>Bear</t>
+  </si>
+  <si>
+    <t>Alice</t>
+  </si>
+  <si>
+    <t>2007</t>
+  </si>
+  <si>
+    <t>Hot</t>
+  </si>
+  <si>
+    <t>Blank</t>
+  </si>
+  <si>
+    <t>Crew</t>
+  </si>
+  <si>
+    <t>Anime</t>
+  </si>
+  <si>
+    <t>Hawaii</t>
+  </si>
+  <si>
+    <t>Joe</t>
+  </si>
+  <si>
+    <t>Shirts</t>
+  </si>
+  <si>
+    <t>Birdhouse</t>
+  </si>
+  <si>
+    <t>Harley-davidson</t>
+  </si>
+  <si>
+    <t>Cafe</t>
+  </si>
+  <si>
+    <t>00's</t>
+  </si>
+  <si>
+    <t>Sports</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Blind</t>
+  </si>
+  <si>
+    <t>Flip</t>
+  </si>
+  <si>
+    <t>Pop</t>
+  </si>
+  <si>
+    <t>Marvel</t>
+  </si>
+  <si>
+    <t>Film</t>
   </si>
   <si>
     <t>Rainbow</t>
   </si>
   <si>
-    <t>Art</t>
-  </si>
-  <si>
-    <t>Brockum</t>
-  </si>
-  <si>
-    <t>Fruit</t>
-  </si>
-  <si>
-    <t>Loom</t>
-  </si>
-  <si>
-    <t>Cotton</t>
-  </si>
-  <si>
-    <t>Dead</t>
-  </si>
-  <si>
-    <t>Movie</t>
-  </si>
-  <si>
-    <t>90s</t>
-  </si>
-  <si>
-    <t>2000</t>
-  </si>
-  <si>
-    <t>1999</t>
-  </si>
-  <si>
-    <t>Mountain</t>
-  </si>
-  <si>
-    <t>Dye</t>
-  </si>
-  <si>
-    <t>Racing</t>
-  </si>
-  <si>
-    <t>Embroidered</t>
-  </si>
-  <si>
-    <t>Crew</t>
-  </si>
-  <si>
-    <t>Neck</t>
-  </si>
-  <si>
-    <t>Pocket</t>
-  </si>
-  <si>
-    <t>Green</t>
-  </si>
-  <si>
-    <t>Star</t>
-  </si>
-  <si>
-    <t>Wars</t>
-  </si>
-  <si>
-    <t>Medium</t>
-  </si>
-  <si>
-    <t>New</t>
-  </si>
-  <si>
-    <t>Disney</t>
-  </si>
-  <si>
-    <t>Rock</t>
-  </si>
-  <si>
-    <t>Adult</t>
-  </si>
-  <si>
-    <t>Skull</t>
-  </si>
-  <si>
-    <t>Nike</t>
-  </si>
-  <si>
-    <t>Center</t>
-  </si>
-  <si>
-    <t>Y2k</t>
-  </si>
-  <si>
-    <t>Baseball</t>
-  </si>
-  <si>
-    <t>Blank</t>
-  </si>
-  <si>
-    <t>Yellow</t>
-  </si>
-  <si>
-    <t>1995</t>
-  </si>
-  <si>
-    <t>Small</t>
-  </si>
-  <si>
-    <t>Music</t>
-  </si>
-  <si>
-    <t>2000s</t>
-  </si>
-  <si>
-    <t>White</t>
-  </si>
-  <si>
-    <t>1989</t>
-  </si>
-  <si>
-    <t>Country</t>
+    <t>Back</t>
+  </si>
+  <si>
+    <t>T-shirts</t>
   </si>
   <si>
     <t>Fit</t>
   </si>
   <si>
-    <t>Marvel</t>
-  </si>
-  <si>
-    <t>Concert</t>
-  </si>
-  <si>
-    <t>Navy</t>
-  </si>
-  <si>
-    <t>90's</t>
-  </si>
-  <si>
-    <t>Harley-davidson</t>
-  </si>
-  <si>
-    <t>Lot</t>
-  </si>
-  <si>
-    <t>Style</t>
-  </si>
-  <si>
-    <t>Shirts</t>
-  </si>
-  <si>
-    <t>1992</t>
-  </si>
-  <si>
-    <t>1991</t>
-  </si>
-  <si>
-    <t>With</t>
-  </si>
-  <si>
-    <t>Harley</t>
-  </si>
-  <si>
-    <t>Davidson</t>
-  </si>
-  <si>
-    <t>Nwt</t>
-  </si>
-  <si>
-    <t>Beach</t>
-  </si>
-  <si>
-    <t>Hawaii</t>
-  </si>
-  <si>
-    <t>|</t>
+    <t>Jam</t>
+  </si>
+  <si>
+    <t>Fits</t>
+  </si>
+  <si>
+    <t>Purple</t>
+  </si>
+  <si>
+    <t>Reseller</t>
   </si>
   <si>
     <t>Hard</t>
-  </si>
-  <si>
-    <t>Cafe</t>
-  </si>
-  <si>
-    <t>Taz</t>
-  </si>
-  <si>
-    <t>1996</t>
-  </si>
-  <si>
-    <t>Sports</t>
-  </si>
-  <si>
-    <t>Aop</t>
-  </si>
-  <si>
-    <t>Tank</t>
-  </si>
-  <si>
-    <t>Top</t>
-  </si>
-  <si>
-    <t>Unisex</t>
-  </si>
-  <si>
-    <t>Gift</t>
-  </si>
-  <si>
-    <t>Brown</t>
-  </si>
-  <si>
-    <t>1990</t>
-  </si>
-  <si>
-    <t>Metal</t>
-  </si>
-  <si>
-    <t>Rap</t>
-  </si>
-  <si>
-    <t>Football</t>
-  </si>
-  <si>
-    <t>Original</t>
-  </si>
-  <si>
-    <t>Band</t>
-  </si>
-  <si>
-    <t>Extra</t>
-  </si>
-  <si>
-    <t>T-shirt,</t>
-  </si>
-  <si>
-    <t>Hip</t>
-  </si>
-  <si>
-    <t>Hop</t>
-  </si>
-  <si>
-    <t>1994</t>
-  </si>
-  <si>
-    <t>Anime</t>
-  </si>
-  <si>
-    <t>Grey</t>
-  </si>
-  <si>
-    <t>Nature</t>
-  </si>
-  <si>
-    <t>1997</t>
-  </si>
-  <si>
-    <t>3xl</t>
-  </si>
-  <si>
-    <t>Distressed</t>
-  </si>
-  <si>
-    <t>Anvil</t>
-  </si>
-  <si>
-    <t>Hanes</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>90’s</t>
-  </si>
-  <si>
-    <t>Wwf</t>
-  </si>
-  <si>
-    <t>Wwe</t>
-  </si>
-  <si>
-    <t>Tag</t>
-  </si>
-  <si>
-    <t>Chicago</t>
-  </si>
-  <si>
-    <t>Ringer</t>
-  </si>
-  <si>
-    <t>Nfl</t>
-  </si>
-  <si>
-    <t>2005</t>
-  </si>
-  <si>
-    <t>Hot</t>
-  </si>
-  <si>
-    <t>Marlboro</t>
-  </si>
-  <si>
-    <t>Space</t>
-  </si>
-  <si>
-    <t>Basketball</t>
-  </si>
-  <si>
-    <t>Jersey</t>
-  </si>
-  <si>
-    <t>Looney</t>
-  </si>
-  <si>
-    <t>Tunes</t>
-  </si>
-  <si>
-    <t>King</t>
-  </si>
-  <si>
-    <t>Back</t>
-  </si>
-  <si>
-    <t>Nascar</t>
-  </si>
-  <si>
-    <t>Florida</t>
-  </si>
-  <si>
-    <t>Punk</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>2001</t>
-  </si>
-  <si>
-    <t>Funny</t>
-  </si>
-  <si>
-    <t>Out</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>1987</t>
-  </si>
-  <si>
-    <t>100%</t>
-  </si>
-  <si>
-    <t>Faded</t>
-  </si>
-  <si>
-    <t>Motorcycle</t>
-  </si>
-  <si>
-    <t>Grateful</t>
-  </si>
-  <si>
-    <t>My</t>
-  </si>
-  <si>
-    <t>Ralph</t>
-  </si>
-  <si>
-    <t>Lauren</t>
-  </si>
-  <si>
-    <t>Orange</t>
-  </si>
-  <si>
-    <t>00s</t>
-  </si>
-  <si>
-    <t>Mc5</t>
-  </si>
-  <si>
-    <t>Sizes</t>
-  </si>
-  <si>
-    <t>Pop</t>
-  </si>
-  <si>
-    <t>Authentic</t>
-  </si>
-  <si>
-    <t>San</t>
-  </si>
-  <si>
-    <t>Weed</t>
-  </si>
-  <si>
-    <t>Culture</t>
-  </si>
-  <si>
-    <t>Screen</t>
-  </si>
-  <si>
-    <t>Stars</t>
-  </si>
-  <si>
-    <t>Polo</t>
-  </si>
-  <si>
-    <t>Ford</t>
   </si>
 </sst>
 </file>
@@ -768,8 +925,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1081,47 +1237,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F182"/>
+  <dimension ref="B1:F234"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="3.53125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.19921875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.46484375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.53125" customWidth="1"/>
+    <col min="4" max="4" width="15.19921875" customWidth="1"/>
+    <col min="5" max="5" width="13.46484375" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="4">
         <v>2</v>
       </c>
     </row>
@@ -1130,17 +1286,17 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>23</v>
+        <v>171</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <f ca="1">TODAY()</f>
-        <v>44784</v>
+        <v>44806</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.45">
@@ -1148,16 +1304,16 @@
         <v>8</v>
       </c>
       <c r="C4">
-        <v>6</v>
+        <v>702</v>
       </c>
       <c r="D4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="9">
-        <v>2</v>
+      <c r="F4" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.45">
@@ -1165,7 +1321,7 @@
         <v>10</v>
       </c>
       <c r="C5">
-        <v>76</v>
+        <v>150</v>
       </c>
       <c r="D5" t="s">
         <v>4</v>
@@ -1176,7 +1332,7 @@
         <v>11</v>
       </c>
       <c r="C6">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
         <v>4</v>
@@ -1187,7 +1343,7 @@
         <v>12</v>
       </c>
       <c r="C7">
-        <v>31</v>
+        <v>237</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
@@ -1198,7 +1354,7 @@
         <v>13</v>
       </c>
       <c r="C8">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
         <v>4</v>
@@ -1209,7 +1365,7 @@
         <v>14</v>
       </c>
       <c r="C9">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="D9" t="s">
         <v>4</v>
@@ -1220,7 +1376,7 @@
         <v>15</v>
       </c>
       <c r="C10">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
         <v>4</v>
@@ -1231,7 +1387,7 @@
         <v>16</v>
       </c>
       <c r="C11">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
         <v>4</v>
@@ -1242,7 +1398,7 @@
         <v>17</v>
       </c>
       <c r="C12">
-        <v>7</v>
+        <v>69</v>
       </c>
       <c r="D12" t="s">
         <v>4</v>
@@ -1253,7 +1409,7 @@
         <v>18</v>
       </c>
       <c r="C13">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="D13" t="s">
         <v>4</v>
@@ -1264,7 +1420,7 @@
         <v>19</v>
       </c>
       <c r="C14">
-        <v>111</v>
+        <v>23</v>
       </c>
       <c r="D14" t="s">
         <v>4</v>
@@ -1275,7 +1431,7 @@
         <v>20</v>
       </c>
       <c r="C15">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D15" t="s">
         <v>4</v>
@@ -1286,7 +1442,7 @@
         <v>21</v>
       </c>
       <c r="C16">
-        <v>13</v>
+        <v>74</v>
       </c>
       <c r="D16" t="s">
         <v>4</v>
@@ -1297,7 +1453,7 @@
         <v>22</v>
       </c>
       <c r="C17">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D17" t="s">
         <v>4</v>
@@ -1308,7 +1464,7 @@
         <v>23</v>
       </c>
       <c r="C18">
-        <v>124</v>
+        <v>51</v>
       </c>
       <c r="D18" t="s">
         <v>4</v>
@@ -1319,7 +1475,7 @@
         <v>24</v>
       </c>
       <c r="C19">
-        <v>10</v>
+        <v>271</v>
       </c>
       <c r="D19" t="s">
         <v>4</v>
@@ -1330,7 +1486,7 @@
         <v>25</v>
       </c>
       <c r="C20">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D20" t="s">
         <v>4</v>
@@ -1341,7 +1497,7 @@
         <v>26</v>
       </c>
       <c r="C21">
-        <v>326</v>
+        <v>17</v>
       </c>
       <c r="D21" t="s">
         <v>4</v>
@@ -1352,7 +1508,7 @@
         <v>27</v>
       </c>
       <c r="C22">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="D22" t="s">
         <v>4</v>
@@ -1363,7 +1519,7 @@
         <v>28</v>
       </c>
       <c r="C23">
-        <v>323</v>
+        <v>290</v>
       </c>
       <c r="D23" t="s">
         <v>4</v>
@@ -1374,7 +1530,7 @@
         <v>29</v>
       </c>
       <c r="C24">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D24" t="s">
         <v>4</v>
@@ -1385,7 +1541,7 @@
         <v>30</v>
       </c>
       <c r="C25">
-        <v>62</v>
+        <v>659</v>
       </c>
       <c r="D25" t="s">
         <v>4</v>
@@ -1396,7 +1552,7 @@
         <v>31</v>
       </c>
       <c r="C26">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="D26" t="s">
         <v>4</v>
@@ -1407,7 +1563,7 @@
         <v>32</v>
       </c>
       <c r="C27">
-        <v>12</v>
+        <v>82</v>
       </c>
       <c r="D27" t="s">
         <v>4</v>
@@ -1418,7 +1574,7 @@
         <v>33</v>
       </c>
       <c r="C28">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="D28" t="s">
         <v>4</v>
@@ -1429,7 +1585,7 @@
         <v>34</v>
       </c>
       <c r="C29">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D29" t="s">
         <v>4</v>
@@ -1440,7 +1596,7 @@
         <v>35</v>
       </c>
       <c r="C30">
-        <v>18</v>
+        <v>304</v>
       </c>
       <c r="D30" t="s">
         <v>4</v>
@@ -1451,7 +1607,7 @@
         <v>36</v>
       </c>
       <c r="C31">
-        <v>149</v>
+        <v>168</v>
       </c>
       <c r="D31" t="s">
         <v>4</v>
@@ -1462,7 +1618,7 @@
         <v>37</v>
       </c>
       <c r="C32">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="D32" t="s">
         <v>4</v>
@@ -1473,7 +1629,7 @@
         <v>38</v>
       </c>
       <c r="C33">
-        <v>129</v>
+        <v>7</v>
       </c>
       <c r="D33" t="s">
         <v>4</v>
@@ -1484,7 +1640,7 @@
         <v>39</v>
       </c>
       <c r="C34">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="D34" t="s">
         <v>4</v>
@@ -1495,7 +1651,7 @@
         <v>40</v>
       </c>
       <c r="C35">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D35" t="s">
         <v>4</v>
@@ -1506,7 +1662,7 @@
         <v>41</v>
       </c>
       <c r="C36">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="D36" t="s">
         <v>4</v>
@@ -1517,7 +1673,7 @@
         <v>42</v>
       </c>
       <c r="C37">
-        <v>33</v>
+        <v>166</v>
       </c>
       <c r="D37" t="s">
         <v>4</v>
@@ -1528,7 +1684,7 @@
         <v>43</v>
       </c>
       <c r="C38">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="D38" t="s">
         <v>4</v>
@@ -1539,7 +1695,7 @@
         <v>44</v>
       </c>
       <c r="C39">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="D39" t="s">
         <v>4</v>
@@ -1550,7 +1706,7 @@
         <v>45</v>
       </c>
       <c r="C40">
-        <v>162</v>
+        <v>11</v>
       </c>
       <c r="D40" t="s">
         <v>4</v>
@@ -1561,7 +1717,7 @@
         <v>46</v>
       </c>
       <c r="C41">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D41" t="s">
         <v>4</v>
@@ -1572,7 +1728,7 @@
         <v>47</v>
       </c>
       <c r="C42">
-        <v>66</v>
+        <v>18</v>
       </c>
       <c r="D42" t="s">
         <v>4</v>
@@ -1583,7 +1739,7 @@
         <v>48</v>
       </c>
       <c r="C43">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="D43" t="s">
         <v>4</v>
@@ -1594,7 +1750,7 @@
         <v>49</v>
       </c>
       <c r="C44">
-        <v>18</v>
+        <v>404</v>
       </c>
       <c r="D44" t="s">
         <v>4</v>
@@ -1605,7 +1761,7 @@
         <v>50</v>
       </c>
       <c r="C45">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="D45" t="s">
         <v>4</v>
@@ -1616,7 +1772,7 @@
         <v>51</v>
       </c>
       <c r="C46">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D46" t="s">
         <v>4</v>
@@ -1627,7 +1783,7 @@
         <v>52</v>
       </c>
       <c r="C47">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D47" t="s">
         <v>4</v>
@@ -1638,7 +1794,7 @@
         <v>53</v>
       </c>
       <c r="C48">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="D48" t="s">
         <v>4</v>
@@ -1649,7 +1805,7 @@
         <v>54</v>
       </c>
       <c r="C49">
-        <v>10</v>
+        <v>77</v>
       </c>
       <c r="D49" t="s">
         <v>4</v>
@@ -1660,7 +1816,7 @@
         <v>55</v>
       </c>
       <c r="C50">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="D50" t="s">
         <v>4</v>
@@ -1671,7 +1827,7 @@
         <v>56</v>
       </c>
       <c r="C51">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D51" t="s">
         <v>4</v>
@@ -1682,7 +1838,7 @@
         <v>57</v>
       </c>
       <c r="C52">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D52" t="s">
         <v>4</v>
@@ -1693,7 +1849,7 @@
         <v>58</v>
       </c>
       <c r="C53">
-        <v>37</v>
+        <v>156</v>
       </c>
       <c r="D53" t="s">
         <v>4</v>
@@ -1704,7 +1860,7 @@
         <v>59</v>
       </c>
       <c r="C54">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="D54" t="s">
         <v>4</v>
@@ -1715,7 +1871,7 @@
         <v>60</v>
       </c>
       <c r="C55">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="D55" t="s">
         <v>4</v>
@@ -1726,7 +1882,7 @@
         <v>61</v>
       </c>
       <c r="C56">
-        <v>200</v>
+        <v>94</v>
       </c>
       <c r="D56" t="s">
         <v>4</v>
@@ -1737,7 +1893,7 @@
         <v>62</v>
       </c>
       <c r="C57">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="D57" t="s">
         <v>4</v>
@@ -1748,7 +1904,7 @@
         <v>63</v>
       </c>
       <c r="C58">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D58" t="s">
         <v>4</v>
@@ -1759,7 +1915,7 @@
         <v>64</v>
       </c>
       <c r="C59">
-        <v>6</v>
+        <v>275</v>
       </c>
       <c r="D59" t="s">
         <v>4</v>
@@ -1770,7 +1926,7 @@
         <v>65</v>
       </c>
       <c r="C60">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D60" t="s">
         <v>4</v>
@@ -1781,7 +1937,7 @@
         <v>66</v>
       </c>
       <c r="C61">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D61" t="s">
         <v>4</v>
@@ -1792,7 +1948,7 @@
         <v>67</v>
       </c>
       <c r="C62">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="D62" t="s">
         <v>4</v>
@@ -1803,7 +1959,7 @@
         <v>68</v>
       </c>
       <c r="C63">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D63" t="s">
         <v>4</v>
@@ -1814,7 +1970,7 @@
         <v>69</v>
       </c>
       <c r="C64">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="D64" t="s">
         <v>4</v>
@@ -1825,7 +1981,7 @@
         <v>70</v>
       </c>
       <c r="C65">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D65" t="s">
         <v>4</v>
@@ -1836,7 +1992,7 @@
         <v>71</v>
       </c>
       <c r="C66">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="D66" t="s">
         <v>4</v>
@@ -1847,7 +2003,7 @@
         <v>72</v>
       </c>
       <c r="C67">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D67" t="s">
         <v>4</v>
@@ -1858,7 +2014,7 @@
         <v>73</v>
       </c>
       <c r="C68">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D68" t="s">
         <v>4</v>
@@ -1869,7 +2025,7 @@
         <v>74</v>
       </c>
       <c r="C69">
-        <v>133</v>
+        <v>88</v>
       </c>
       <c r="D69" t="s">
         <v>4</v>
@@ -1880,7 +2036,7 @@
         <v>75</v>
       </c>
       <c r="C70">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D70" t="s">
         <v>4</v>
@@ -1891,7 +2047,7 @@
         <v>76</v>
       </c>
       <c r="C71">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D71" t="s">
         <v>4</v>
@@ -1902,7 +2058,7 @@
         <v>77</v>
       </c>
       <c r="C72">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="D72" t="s">
         <v>4</v>
@@ -1913,7 +2069,7 @@
         <v>78</v>
       </c>
       <c r="C73">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="D73" t="s">
         <v>4</v>
@@ -1935,7 +2091,7 @@
         <v>80</v>
       </c>
       <c r="C75">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="D75" t="s">
         <v>4</v>
@@ -1946,7 +2102,7 @@
         <v>81</v>
       </c>
       <c r="C76">
-        <v>6</v>
+        <v>102</v>
       </c>
       <c r="D76" t="s">
         <v>4</v>
@@ -1957,7 +2113,7 @@
         <v>82</v>
       </c>
       <c r="C77">
-        <v>38</v>
+        <v>180</v>
       </c>
       <c r="D77" t="s">
         <v>4</v>
@@ -1968,7 +2124,7 @@
         <v>83</v>
       </c>
       <c r="C78">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D78" t="s">
         <v>4</v>
@@ -1979,7 +2135,7 @@
         <v>84</v>
       </c>
       <c r="C79">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="D79" t="s">
         <v>4</v>
@@ -1990,7 +2146,7 @@
         <v>85</v>
       </c>
       <c r="C80">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="D80" t="s">
         <v>4</v>
@@ -2001,7 +2157,7 @@
         <v>86</v>
       </c>
       <c r="C81">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="D81" t="s">
         <v>4</v>
@@ -2012,7 +2168,7 @@
         <v>87</v>
       </c>
       <c r="C82">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D82" t="s">
         <v>4</v>
@@ -2023,7 +2179,7 @@
         <v>88</v>
       </c>
       <c r="C83">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D83" t="s">
         <v>4</v>
@@ -2034,7 +2190,7 @@
         <v>89</v>
       </c>
       <c r="C84">
-        <v>9</v>
+        <v>107</v>
       </c>
       <c r="D84" t="s">
         <v>4</v>
@@ -2045,7 +2201,7 @@
         <v>90</v>
       </c>
       <c r="C85">
-        <v>76</v>
+        <v>22</v>
       </c>
       <c r="D85" t="s">
         <v>4</v>
@@ -2056,7 +2212,7 @@
         <v>91</v>
       </c>
       <c r="C86">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D86" t="s">
         <v>4</v>
@@ -2067,7 +2223,7 @@
         <v>92</v>
       </c>
       <c r="C87">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="D87" t="s">
         <v>4</v>
@@ -2078,7 +2234,7 @@
         <v>93</v>
       </c>
       <c r="C88">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D88" t="s">
         <v>4</v>
@@ -2089,7 +2245,7 @@
         <v>94</v>
       </c>
       <c r="C89">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D89" t="s">
         <v>4</v>
@@ -2100,7 +2256,7 @@
         <v>95</v>
       </c>
       <c r="C90">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="D90" t="s">
         <v>4</v>
@@ -2111,7 +2267,7 @@
         <v>96</v>
       </c>
       <c r="C91">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D91" t="s">
         <v>4</v>
@@ -2122,7 +2278,7 @@
         <v>97</v>
       </c>
       <c r="C92">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D92" t="s">
         <v>4</v>
@@ -2133,7 +2289,7 @@
         <v>98</v>
       </c>
       <c r="C93">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D93" t="s">
         <v>4</v>
@@ -2144,7 +2300,7 @@
         <v>99</v>
       </c>
       <c r="C94">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D94" t="s">
         <v>4</v>
@@ -2155,7 +2311,7 @@
         <v>100</v>
       </c>
       <c r="C95">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D95" t="s">
         <v>4</v>
@@ -2166,7 +2322,7 @@
         <v>101</v>
       </c>
       <c r="C96">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D96" t="s">
         <v>4</v>
@@ -2177,7 +2333,7 @@
         <v>102</v>
       </c>
       <c r="C97">
-        <v>24</v>
+        <v>142</v>
       </c>
       <c r="D97" t="s">
         <v>4</v>
@@ -2188,7 +2344,7 @@
         <v>103</v>
       </c>
       <c r="C98">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D98" t="s">
         <v>4</v>
@@ -2199,7 +2355,7 @@
         <v>104</v>
       </c>
       <c r="C99">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D99" t="s">
         <v>4</v>
@@ -2210,7 +2366,7 @@
         <v>105</v>
       </c>
       <c r="C100">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="D100" t="s">
         <v>4</v>
@@ -2221,7 +2377,7 @@
         <v>106</v>
       </c>
       <c r="C101">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D101" t="s">
         <v>4</v>
@@ -2232,7 +2388,7 @@
         <v>107</v>
       </c>
       <c r="C102">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D102" t="s">
         <v>4</v>
@@ -2243,7 +2399,7 @@
         <v>108</v>
       </c>
       <c r="C103">
-        <v>9</v>
+        <v>115</v>
       </c>
       <c r="D103" t="s">
         <v>4</v>
@@ -2254,7 +2410,7 @@
         <v>109</v>
       </c>
       <c r="C104">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D104" t="s">
         <v>4</v>
@@ -2265,7 +2421,7 @@
         <v>110</v>
       </c>
       <c r="C105">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="D105" t="s">
         <v>4</v>
@@ -2276,7 +2432,7 @@
         <v>111</v>
       </c>
       <c r="C106">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="D106" t="s">
         <v>4</v>
@@ -2287,7 +2443,7 @@
         <v>112</v>
       </c>
       <c r="C107">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D107" t="s">
         <v>4</v>
@@ -2298,7 +2454,7 @@
         <v>113</v>
       </c>
       <c r="C108">
-        <v>6</v>
+        <v>57</v>
       </c>
       <c r="D108" t="s">
         <v>4</v>
@@ -2309,7 +2465,7 @@
         <v>114</v>
       </c>
       <c r="C109">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="D109" t="s">
         <v>4</v>
@@ -2320,7 +2476,7 @@
         <v>115</v>
       </c>
       <c r="C110">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D110" t="s">
         <v>4</v>
@@ -2331,7 +2487,7 @@
         <v>116</v>
       </c>
       <c r="C111">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="D111" t="s">
         <v>4</v>
@@ -2342,7 +2498,7 @@
         <v>117</v>
       </c>
       <c r="C112">
-        <v>19</v>
+        <v>95</v>
       </c>
       <c r="D112" t="s">
         <v>4</v>
@@ -2353,7 +2509,7 @@
         <v>118</v>
       </c>
       <c r="C113">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="D113" t="s">
         <v>4</v>
@@ -2364,7 +2520,7 @@
         <v>119</v>
       </c>
       <c r="C114">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="D114" t="s">
         <v>4</v>
@@ -2375,7 +2531,7 @@
         <v>120</v>
       </c>
       <c r="C115">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D115" t="s">
         <v>4</v>
@@ -2386,7 +2542,7 @@
         <v>121</v>
       </c>
       <c r="C116">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="D116" t="s">
         <v>4</v>
@@ -2397,7 +2553,7 @@
         <v>122</v>
       </c>
       <c r="C117">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="D117" t="s">
         <v>4</v>
@@ -2408,7 +2564,7 @@
         <v>123</v>
       </c>
       <c r="C118">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D118" t="s">
         <v>4</v>
@@ -2419,7 +2575,7 @@
         <v>124</v>
       </c>
       <c r="C119">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D119" t="s">
         <v>4</v>
@@ -2430,7 +2586,7 @@
         <v>125</v>
       </c>
       <c r="C120">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D120" t="s">
         <v>4</v>
@@ -2441,7 +2597,7 @@
         <v>126</v>
       </c>
       <c r="C121">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="D121" t="s">
         <v>4</v>
@@ -2452,7 +2608,7 @@
         <v>127</v>
       </c>
       <c r="C122">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="D122" t="s">
         <v>4</v>
@@ -2463,7 +2619,7 @@
         <v>128</v>
       </c>
       <c r="C123">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D123" t="s">
         <v>4</v>
@@ -2474,7 +2630,7 @@
         <v>129</v>
       </c>
       <c r="C124">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D124" t="s">
         <v>4</v>
@@ -2485,7 +2641,7 @@
         <v>130</v>
       </c>
       <c r="C125">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="D125" t="s">
         <v>4</v>
@@ -2496,7 +2652,7 @@
         <v>131</v>
       </c>
       <c r="C126">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D126" t="s">
         <v>4</v>
@@ -2507,7 +2663,7 @@
         <v>132</v>
       </c>
       <c r="C127">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D127" t="s">
         <v>4</v>
@@ -2518,7 +2674,7 @@
         <v>133</v>
       </c>
       <c r="C128">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D128" t="s">
         <v>4</v>
@@ -2540,7 +2696,7 @@
         <v>135</v>
       </c>
       <c r="C130">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="D130" t="s">
         <v>4</v>
@@ -2551,7 +2707,7 @@
         <v>136</v>
       </c>
       <c r="C131">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="D131" t="s">
         <v>4</v>
@@ -2562,7 +2718,7 @@
         <v>137</v>
       </c>
       <c r="C132">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D132" t="s">
         <v>4</v>
@@ -2573,7 +2729,7 @@
         <v>138</v>
       </c>
       <c r="C133">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D133" t="s">
         <v>4</v>
@@ -2584,7 +2740,7 @@
         <v>139</v>
       </c>
       <c r="C134">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D134" t="s">
         <v>4</v>
@@ -2595,7 +2751,7 @@
         <v>140</v>
       </c>
       <c r="C135">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D135" t="s">
         <v>4</v>
@@ -2606,7 +2762,7 @@
         <v>141</v>
       </c>
       <c r="C136">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="D136" t="s">
         <v>4</v>
@@ -2617,7 +2773,7 @@
         <v>142</v>
       </c>
       <c r="C137">
-        <v>13</v>
+        <v>112</v>
       </c>
       <c r="D137" t="s">
         <v>4</v>
@@ -2628,7 +2784,7 @@
         <v>143</v>
       </c>
       <c r="C138">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="D138" t="s">
         <v>4</v>
@@ -2639,7 +2795,7 @@
         <v>144</v>
       </c>
       <c r="C139">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="D139" t="s">
         <v>4</v>
@@ -2650,7 +2806,7 @@
         <v>145</v>
       </c>
       <c r="C140">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D140" t="s">
         <v>4</v>
@@ -2661,7 +2817,7 @@
         <v>146</v>
       </c>
       <c r="C141">
-        <v>6</v>
+        <v>117</v>
       </c>
       <c r="D141" t="s">
         <v>4</v>
@@ -2672,7 +2828,7 @@
         <v>147</v>
       </c>
       <c r="C142">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D142" t="s">
         <v>4</v>
@@ -2683,7 +2839,7 @@
         <v>148</v>
       </c>
       <c r="C143">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D143" t="s">
         <v>4</v>
@@ -2694,7 +2850,7 @@
         <v>149</v>
       </c>
       <c r="C144">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D144" t="s">
         <v>4</v>
@@ -2705,7 +2861,7 @@
         <v>150</v>
       </c>
       <c r="C145">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D145" t="s">
         <v>4</v>
@@ -2716,7 +2872,7 @@
         <v>151</v>
       </c>
       <c r="C146">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D146" t="s">
         <v>4</v>
@@ -2727,7 +2883,7 @@
         <v>152</v>
       </c>
       <c r="C147">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D147" t="s">
         <v>4</v>
@@ -2738,9 +2894,9 @@
         <v>153</v>
       </c>
       <c r="C148">
-        <v>13</v>
-      </c>
-      <c r="D148" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D148" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2749,9 +2905,9 @@
         <v>154</v>
       </c>
       <c r="C149">
-        <v>17</v>
-      </c>
-      <c r="D149" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D149" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2760,9 +2916,9 @@
         <v>155</v>
       </c>
       <c r="C150">
-        <v>8</v>
-      </c>
-      <c r="D150" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D150" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2771,9 +2927,9 @@
         <v>156</v>
       </c>
       <c r="C151">
-        <v>8</v>
-      </c>
-      <c r="D151" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D151" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2782,9 +2938,9 @@
         <v>157</v>
       </c>
       <c r="C152">
-        <v>11</v>
-      </c>
-      <c r="D152" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D152" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2793,9 +2949,9 @@
         <v>158</v>
       </c>
       <c r="C153">
-        <v>11</v>
-      </c>
-      <c r="D153" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D153" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2804,9 +2960,9 @@
         <v>159</v>
       </c>
       <c r="C154">
-        <v>18</v>
-      </c>
-      <c r="D154" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D154" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2815,9 +2971,9 @@
         <v>160</v>
       </c>
       <c r="C155">
-        <v>10</v>
-      </c>
-      <c r="D155" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D155" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2826,9 +2982,9 @@
         <v>161</v>
       </c>
       <c r="C156">
-        <v>6</v>
-      </c>
-      <c r="D156" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D156" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2837,9 +2993,9 @@
         <v>162</v>
       </c>
       <c r="C157">
-        <v>11</v>
-      </c>
-      <c r="D157" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D157" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2848,9 +3004,9 @@
         <v>163</v>
       </c>
       <c r="C158">
-        <v>7</v>
-      </c>
-      <c r="D158" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D158" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2859,9 +3015,9 @@
         <v>164</v>
       </c>
       <c r="C159">
-        <v>8</v>
-      </c>
-      <c r="D159" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D159" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2870,9 +3026,9 @@
         <v>165</v>
       </c>
       <c r="C160">
-        <v>14</v>
-      </c>
-      <c r="D160" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D160" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2881,9 +3037,9 @@
         <v>166</v>
       </c>
       <c r="C161">
-        <v>9</v>
-      </c>
-      <c r="D161" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D161" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2892,9 +3048,9 @@
         <v>167</v>
       </c>
       <c r="C162">
-        <v>11</v>
-      </c>
-      <c r="D162" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D162" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2903,9 +3059,9 @@
         <v>168</v>
       </c>
       <c r="C163">
-        <v>7</v>
-      </c>
-      <c r="D163" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D163" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2914,9 +3070,9 @@
         <v>169</v>
       </c>
       <c r="C164">
-        <v>17</v>
-      </c>
-      <c r="D164" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D164" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2925,9 +3081,9 @@
         <v>170</v>
       </c>
       <c r="C165">
-        <v>17</v>
-      </c>
-      <c r="D165" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D165" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2936,9 +3092,9 @@
         <v>171</v>
       </c>
       <c r="C166">
-        <v>12</v>
-      </c>
-      <c r="D166" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D166" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2947,9 +3103,9 @@
         <v>172</v>
       </c>
       <c r="C167">
-        <v>11</v>
-      </c>
-      <c r="D167" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D167" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2958,9 +3114,9 @@
         <v>173</v>
       </c>
       <c r="C168">
-        <v>9</v>
-      </c>
-      <c r="D168" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D168" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2969,9 +3125,9 @@
         <v>174</v>
       </c>
       <c r="C169">
-        <v>9</v>
-      </c>
-      <c r="D169" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D169" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2980,9 +3136,9 @@
         <v>175</v>
       </c>
       <c r="C170">
-        <v>10</v>
-      </c>
-      <c r="D170" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D170" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2991,9 +3147,9 @@
         <v>176</v>
       </c>
       <c r="C171">
-        <v>8</v>
-      </c>
-      <c r="D171" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D171" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3002,9 +3158,9 @@
         <v>177</v>
       </c>
       <c r="C172">
-        <v>6</v>
-      </c>
-      <c r="D172" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D172" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3013,9 +3169,9 @@
         <v>178</v>
       </c>
       <c r="C173">
-        <v>6</v>
-      </c>
-      <c r="D173" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D173" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3024,9 +3180,9 @@
         <v>179</v>
       </c>
       <c r="C174">
-        <v>8</v>
-      </c>
-      <c r="D174" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D174" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3035,9 +3191,9 @@
         <v>180</v>
       </c>
       <c r="C175">
-        <v>9</v>
-      </c>
-      <c r="D175" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D175" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3046,9 +3202,9 @@
         <v>181</v>
       </c>
       <c r="C176">
-        <v>6</v>
-      </c>
-      <c r="D176" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D176" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3057,9 +3213,9 @@
         <v>182</v>
       </c>
       <c r="C177">
-        <v>7</v>
-      </c>
-      <c r="D177" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D177" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3068,9 +3224,9 @@
         <v>183</v>
       </c>
       <c r="C178">
-        <v>7</v>
-      </c>
-      <c r="D178" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D178" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3079,9 +3235,9 @@
         <v>184</v>
       </c>
       <c r="C179">
-        <v>9</v>
-      </c>
-      <c r="D179" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D179" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3090,9 +3246,9 @@
         <v>185</v>
       </c>
       <c r="C180">
-        <v>12</v>
-      </c>
-      <c r="D180" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D180" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3101,9 +3257,9 @@
         <v>186</v>
       </c>
       <c r="C181">
-        <v>12</v>
-      </c>
-      <c r="D181" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D181" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3112,9 +3268,581 @@
         <v>187</v>
       </c>
       <c r="C182">
+        <v>61</v>
+      </c>
+      <c r="D182" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="183" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B183" t="s">
+        <v>188</v>
+      </c>
+      <c r="C183">
+        <v>23</v>
+      </c>
+      <c r="D183" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="184" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B184" t="s">
+        <v>189</v>
+      </c>
+      <c r="C184">
+        <v>18</v>
+      </c>
+      <c r="D184" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="185" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B185" t="s">
+        <v>190</v>
+      </c>
+      <c r="C185">
+        <v>7</v>
+      </c>
+      <c r="D185" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="186" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B186" t="s">
+        <v>191</v>
+      </c>
+      <c r="C186">
+        <v>29</v>
+      </c>
+      <c r="D186" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="187" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B187" t="s">
+        <v>192</v>
+      </c>
+      <c r="C187">
+        <v>31</v>
+      </c>
+      <c r="D187" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="188" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B188" t="s">
+        <v>193</v>
+      </c>
+      <c r="C188">
+        <v>20</v>
+      </c>
+      <c r="D188" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="189" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B189" t="s">
+        <v>194</v>
+      </c>
+      <c r="C189">
+        <v>6</v>
+      </c>
+      <c r="D189" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="190" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B190" t="s">
+        <v>195</v>
+      </c>
+      <c r="C190">
         <v>8</v>
       </c>
-      <c r="D182" s="1" t="s">
+      <c r="D190" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="191" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B191" t="s">
+        <v>196</v>
+      </c>
+      <c r="C191">
+        <v>7</v>
+      </c>
+      <c r="D191" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="192" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B192" t="s">
+        <v>197</v>
+      </c>
+      <c r="C192">
+        <v>10</v>
+      </c>
+      <c r="D192" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="193" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B193" t="s">
+        <v>198</v>
+      </c>
+      <c r="C193">
+        <v>13</v>
+      </c>
+      <c r="D193" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="194" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B194" t="s">
+        <v>199</v>
+      </c>
+      <c r="C194">
+        <v>7</v>
+      </c>
+      <c r="D194" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="195" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B195" t="s">
+        <v>200</v>
+      </c>
+      <c r="C195">
+        <v>21</v>
+      </c>
+      <c r="D195" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="196" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B196" t="s">
+        <v>201</v>
+      </c>
+      <c r="C196">
+        <v>10</v>
+      </c>
+      <c r="D196" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="197" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B197" t="s">
+        <v>202</v>
+      </c>
+      <c r="C197">
+        <v>13</v>
+      </c>
+      <c r="D197" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="198" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B198" t="s">
+        <v>203</v>
+      </c>
+      <c r="C198">
+        <v>14</v>
+      </c>
+      <c r="D198" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="199" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B199" t="s">
+        <v>204</v>
+      </c>
+      <c r="C199">
+        <v>18</v>
+      </c>
+      <c r="D199" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="200" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B200" t="s">
+        <v>205</v>
+      </c>
+      <c r="C200">
+        <v>13</v>
+      </c>
+      <c r="D200" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="201" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B201" t="s">
+        <v>206</v>
+      </c>
+      <c r="C201">
+        <v>33</v>
+      </c>
+      <c r="D201" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="202" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B202" t="s">
+        <v>207</v>
+      </c>
+      <c r="C202">
+        <v>28</v>
+      </c>
+      <c r="D202" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="203" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B203" t="s">
+        <v>208</v>
+      </c>
+      <c r="C203">
+        <v>17</v>
+      </c>
+      <c r="D203" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="204" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B204" t="s">
+        <v>209</v>
+      </c>
+      <c r="C204">
+        <v>22</v>
+      </c>
+      <c r="D204" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="205" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B205" t="s">
+        <v>210</v>
+      </c>
+      <c r="C205">
+        <v>10</v>
+      </c>
+      <c r="D205" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="206" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B206" t="s">
+        <v>211</v>
+      </c>
+      <c r="C206">
+        <v>6</v>
+      </c>
+      <c r="D206" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="207" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B207" t="s">
+        <v>212</v>
+      </c>
+      <c r="C207">
+        <v>7</v>
+      </c>
+      <c r="D207" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="208" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B208" t="s">
+        <v>213</v>
+      </c>
+      <c r="C208">
+        <v>19</v>
+      </c>
+      <c r="D208" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="209" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B209" t="s">
+        <v>214</v>
+      </c>
+      <c r="C209">
+        <v>16</v>
+      </c>
+      <c r="D209" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="210" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B210" t="s">
+        <v>215</v>
+      </c>
+      <c r="C210">
+        <v>30</v>
+      </c>
+      <c r="D210" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="211" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B211" t="s">
+        <v>216</v>
+      </c>
+      <c r="C211">
+        <v>8</v>
+      </c>
+      <c r="D211" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="212" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B212" t="s">
+        <v>217</v>
+      </c>
+      <c r="C212">
+        <v>18</v>
+      </c>
+      <c r="D212" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="213" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B213" t="s">
+        <v>218</v>
+      </c>
+      <c r="C213">
+        <v>8</v>
+      </c>
+      <c r="D213" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="214" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B214" t="s">
+        <v>219</v>
+      </c>
+      <c r="C214">
+        <v>20</v>
+      </c>
+      <c r="D214" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="215" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B215" t="s">
+        <v>220</v>
+      </c>
+      <c r="C215">
+        <v>12</v>
+      </c>
+      <c r="D215" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="216" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B216" t="s">
+        <v>221</v>
+      </c>
+      <c r="C216">
+        <v>9</v>
+      </c>
+      <c r="D216" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="217" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B217" t="s">
+        <v>222</v>
+      </c>
+      <c r="C217">
+        <v>21</v>
+      </c>
+      <c r="D217" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="218" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B218" t="s">
+        <v>223</v>
+      </c>
+      <c r="C218">
+        <v>8</v>
+      </c>
+      <c r="D218" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="219" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B219" t="s">
+        <v>224</v>
+      </c>
+      <c r="C219">
+        <v>15</v>
+      </c>
+      <c r="D219" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="220" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B220" t="s">
+        <v>225</v>
+      </c>
+      <c r="C220">
+        <v>9</v>
+      </c>
+      <c r="D220" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="221" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B221" t="s">
+        <v>226</v>
+      </c>
+      <c r="C221">
+        <v>12</v>
+      </c>
+      <c r="D221" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="222" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B222" t="s">
+        <v>227</v>
+      </c>
+      <c r="C222">
+        <v>9</v>
+      </c>
+      <c r="D222" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="223" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B223" t="s">
+        <v>228</v>
+      </c>
+      <c r="C223">
+        <v>13</v>
+      </c>
+      <c r="D223" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="224" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B224" t="s">
+        <v>229</v>
+      </c>
+      <c r="C224">
+        <v>18</v>
+      </c>
+      <c r="D224" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="225" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B225" t="s">
+        <v>230</v>
+      </c>
+      <c r="C225">
+        <v>6</v>
+      </c>
+      <c r="D225" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="226" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B226" t="s">
+        <v>231</v>
+      </c>
+      <c r="C226">
+        <v>11</v>
+      </c>
+      <c r="D226" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="227" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B227" t="s">
+        <v>232</v>
+      </c>
+      <c r="C227">
+        <v>18</v>
+      </c>
+      <c r="D227" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="228" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B228" t="s">
+        <v>233</v>
+      </c>
+      <c r="C228">
+        <v>8</v>
+      </c>
+      <c r="D228" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="229" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B229" t="s">
+        <v>234</v>
+      </c>
+      <c r="C229">
+        <v>9</v>
+      </c>
+      <c r="D229" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="230" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B230" t="s">
+        <v>235</v>
+      </c>
+      <c r="C230">
+        <v>8</v>
+      </c>
+      <c r="D230" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="231" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B231" t="s">
+        <v>236</v>
+      </c>
+      <c r="C231">
+        <v>7</v>
+      </c>
+      <c r="D231" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="232" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B232" t="s">
+        <v>237</v>
+      </c>
+      <c r="C232">
+        <v>8</v>
+      </c>
+      <c r="D232" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="233" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B233" t="s">
+        <v>238</v>
+      </c>
+      <c r="C233">
+        <v>6</v>
+      </c>
+      <c r="D233" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="234" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B234" t="s">
+        <v>239</v>
+      </c>
+      <c r="C234">
+        <v>20</v>
+      </c>
+      <c r="D234" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>